<commit_message>
szamitogep leiras hozzaadas es gantt-diagram kitoltes
</commit_message>
<xml_diff>
--- a/docs/M1/gantt-diagram.xlsx
+++ b/docs/M1/gantt-diagram.xlsx
@@ -264,19 +264,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
@@ -689,7 +686,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -703,7 +700,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -805,11 +802,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="11" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="11" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -841,7 +838,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -869,7 +866,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -885,7 +882,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -901,7 +898,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -912,12 +909,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="17" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="17" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -937,7 +930,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="18" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="18" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -949,11 +942,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="18" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="19" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -969,7 +962,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="20" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="20" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -981,7 +974,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1049,12 +1042,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1083,12 +1072,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1117,12 +1102,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1151,12 +1132,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1164,12 +1141,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1219,12 +1192,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1253,12 +1222,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1287,12 +1252,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1321,12 +1282,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1355,12 +1312,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1389,12 +1342,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1423,12 +1372,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1457,12 +1402,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1491,12 +1432,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1525,12 +1462,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1559,12 +1492,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1593,12 +1522,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1627,12 +1552,8 @@
     </dxf>
     <dxf>
       <border diagonalUp="false" diagonalDown="false">
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
+        <left style="thin"/>
+        <right style="thin"/>
         <top/>
         <bottom/>
         <diagonal/>
@@ -1703,7 +1624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -1712,7 +1633,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="Q14" activeCellId="0" sqref="Q14"/>
+      <selection pane="bottomLeft" activeCell="U9" activeCellId="0" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="30" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2527,7 +2448,7 @@
       <c r="R9" s="33"/>
       <c r="S9" s="39"/>
       <c r="T9" s="39"/>
-      <c r="U9" s="33"/>
+      <c r="U9" s="11"/>
       <c r="V9" s="33"/>
       <c r="W9" s="33"/>
       <c r="X9" s="33"/>
@@ -2806,7 +2727,7 @@
       <c r="V12" s="33"/>
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
-      <c r="Y12" s="52"/>
+      <c r="Y12" s="0"/>
       <c r="Z12" s="39"/>
       <c r="AA12" s="39"/>
       <c r="AB12" s="33"/>
@@ -3000,7 +2921,7 @@
       <c r="AB14" s="33"/>
       <c r="AC14" s="33"/>
       <c r="AD14" s="33"/>
-      <c r="AE14" s="52"/>
+      <c r="AE14" s="0"/>
       <c r="AF14" s="33"/>
       <c r="AG14" s="39"/>
       <c r="AH14" s="39"/>
@@ -3283,7 +3204,7 @@
       <c r="AC17" s="33"/>
       <c r="AD17" s="33"/>
       <c r="AE17" s="33"/>
-      <c r="AF17" s="52"/>
+      <c r="AF17" s="0"/>
       <c r="AG17" s="39"/>
       <c r="AH17" s="39"/>
       <c r="AI17" s="33"/>
@@ -3338,105 +3259,105 @@
     </row>
     <row r="18" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="38"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="57"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="57"/>
-      <c r="R18" s="57"/>
-      <c r="S18" s="57"/>
-      <c r="T18" s="57"/>
-      <c r="U18" s="57"/>
-      <c r="V18" s="57"/>
-      <c r="W18" s="57"/>
-      <c r="X18" s="57"/>
-      <c r="Y18" s="57"/>
-      <c r="Z18" s="57"/>
-      <c r="AA18" s="57"/>
-      <c r="AB18" s="57"/>
-      <c r="AC18" s="57"/>
-      <c r="AD18" s="57"/>
-      <c r="AE18" s="57"/>
-      <c r="AF18" s="57"/>
-      <c r="AG18" s="57"/>
-      <c r="AH18" s="57"/>
-      <c r="AI18" s="57"/>
-      <c r="AJ18" s="57"/>
-      <c r="AK18" s="57"/>
-      <c r="AL18" s="57"/>
-      <c r="AM18" s="57"/>
-      <c r="AN18" s="57"/>
-      <c r="AO18" s="57"/>
-      <c r="AP18" s="57"/>
-      <c r="AQ18" s="57"/>
-      <c r="AR18" s="57"/>
-      <c r="AS18" s="57"/>
-      <c r="AT18" s="57"/>
-      <c r="AU18" s="57"/>
-      <c r="AV18" s="57"/>
-      <c r="AW18" s="57"/>
-      <c r="AX18" s="57"/>
-      <c r="AY18" s="57"/>
-      <c r="AZ18" s="57"/>
-      <c r="BA18" s="57"/>
-      <c r="BB18" s="57"/>
-      <c r="BC18" s="57"/>
-      <c r="BD18" s="57"/>
-      <c r="BE18" s="57"/>
-      <c r="BF18" s="57"/>
-      <c r="BG18" s="57"/>
-      <c r="BH18" s="57"/>
-      <c r="BI18" s="57"/>
-      <c r="BJ18" s="57"/>
-      <c r="BK18" s="57"/>
-      <c r="BL18" s="57"/>
-      <c r="BM18" s="57"/>
-      <c r="BN18" s="57"/>
-      <c r="BO18" s="57"/>
-      <c r="BP18" s="57"/>
-      <c r="BQ18" s="57"/>
-      <c r="BR18" s="57"/>
-      <c r="BS18" s="57"/>
-      <c r="BT18" s="57"/>
-      <c r="BU18" s="57"/>
-      <c r="BV18" s="57"/>
-      <c r="BW18" s="57"/>
-      <c r="BX18" s="57"/>
-      <c r="BY18" s="57"/>
-      <c r="BZ18" s="57"/>
-      <c r="CA18" s="57"/>
-      <c r="CB18" s="57"/>
-      <c r="CC18" s="57"/>
-      <c r="CD18" s="57"/>
-      <c r="CE18" s="57"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+      <c r="U18" s="56"/>
+      <c r="V18" s="56"/>
+      <c r="W18" s="56"/>
+      <c r="X18" s="56"/>
+      <c r="Y18" s="56"/>
+      <c r="Z18" s="56"/>
+      <c r="AA18" s="56"/>
+      <c r="AB18" s="56"/>
+      <c r="AC18" s="56"/>
+      <c r="AD18" s="56"/>
+      <c r="AE18" s="56"/>
+      <c r="AF18" s="56"/>
+      <c r="AG18" s="56"/>
+      <c r="AH18" s="56"/>
+      <c r="AI18" s="56"/>
+      <c r="AJ18" s="56"/>
+      <c r="AK18" s="56"/>
+      <c r="AL18" s="56"/>
+      <c r="AM18" s="56"/>
+      <c r="AN18" s="56"/>
+      <c r="AO18" s="56"/>
+      <c r="AP18" s="56"/>
+      <c r="AQ18" s="56"/>
+      <c r="AR18" s="56"/>
+      <c r="AS18" s="56"/>
+      <c r="AT18" s="56"/>
+      <c r="AU18" s="56"/>
+      <c r="AV18" s="56"/>
+      <c r="AW18" s="56"/>
+      <c r="AX18" s="56"/>
+      <c r="AY18" s="56"/>
+      <c r="AZ18" s="56"/>
+      <c r="BA18" s="56"/>
+      <c r="BB18" s="56"/>
+      <c r="BC18" s="56"/>
+      <c r="BD18" s="56"/>
+      <c r="BE18" s="56"/>
+      <c r="BF18" s="56"/>
+      <c r="BG18" s="56"/>
+      <c r="BH18" s="56"/>
+      <c r="BI18" s="56"/>
+      <c r="BJ18" s="56"/>
+      <c r="BK18" s="56"/>
+      <c r="BL18" s="56"/>
+      <c r="BM18" s="56"/>
+      <c r="BN18" s="56"/>
+      <c r="BO18" s="56"/>
+      <c r="BP18" s="56"/>
+      <c r="BQ18" s="56"/>
+      <c r="BR18" s="56"/>
+      <c r="BS18" s="56"/>
+      <c r="BT18" s="56"/>
+      <c r="BU18" s="56"/>
+      <c r="BV18" s="56"/>
+      <c r="BW18" s="56"/>
+      <c r="BX18" s="56"/>
+      <c r="BY18" s="56"/>
+      <c r="BZ18" s="56"/>
+      <c r="CA18" s="56"/>
+      <c r="CB18" s="56"/>
+      <c r="CC18" s="56"/>
+      <c r="CD18" s="56"/>
+      <c r="CE18" s="56"/>
     </row>
     <row r="19" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="60" t="n">
+      <c r="D19" s="59" t="n">
         <v>44492</v>
       </c>
-      <c r="E19" s="60" t="n">
+      <c r="E19" s="59" t="n">
         <f aca="false">D19+4</f>
         <v>44496</v>
       </c>
@@ -3521,16 +3442,16 @@
     </row>
     <row r="20" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="60" t="n">
+      <c r="D20" s="59" t="n">
         <v>44489</v>
       </c>
-      <c r="E20" s="60" t="n">
+      <c r="E20" s="59" t="n">
         <f aca="false">D20+3</f>
         <v>44492</v>
       </c>
@@ -3615,16 +3536,16 @@
     </row>
     <row r="21" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="60" t="n">
+      <c r="D21" s="59" t="n">
         <v>44488</v>
       </c>
-      <c r="E21" s="60" t="n">
+      <c r="E21" s="59" t="n">
         <f aca="false">D21+2</f>
         <v>44490</v>
       </c>
@@ -3709,16 +3630,16 @@
     </row>
     <row r="22" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="60" t="n">
+      <c r="D22" s="59" t="n">
         <v>44497</v>
       </c>
-      <c r="E22" s="60" t="n">
+      <c r="E22" s="59" t="n">
         <f aca="false">D22+9</f>
         <v>44506</v>
       </c>
@@ -3803,16 +3724,16 @@
     </row>
     <row r="23" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="60" t="n">
+      <c r="D23" s="59" t="n">
         <v>44501</v>
       </c>
-      <c r="E23" s="60" t="n">
+      <c r="E23" s="59" t="n">
         <f aca="false">D23+2</f>
         <v>44503</v>
       </c>
@@ -3897,16 +3818,16 @@
     </row>
     <row r="24" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="60" t="n">
+      <c r="D24" s="59" t="n">
         <v>44494</v>
       </c>
-      <c r="E24" s="60" t="n">
+      <c r="E24" s="59" t="n">
         <f aca="false">D24+3</f>
         <v>44497</v>
       </c>
@@ -3991,16 +3912,16 @@
     </row>
     <row r="25" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="60" t="n">
+      <c r="D25" s="59" t="n">
         <v>44497</v>
       </c>
-      <c r="E25" s="60" t="n">
+      <c r="E25" s="59" t="n">
         <f aca="false">D25+3</f>
         <v>44500</v>
       </c>
@@ -4085,16 +4006,16 @@
     </row>
     <row r="26" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="60" t="n">
+      <c r="D26" s="59" t="n">
         <v>44495</v>
       </c>
-      <c r="E26" s="60" t="n">
+      <c r="E26" s="59" t="n">
         <f aca="false">D26+2</f>
         <v>44497</v>
       </c>
@@ -4179,16 +4100,16 @@
     </row>
     <row r="27" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="59" t="s">
+      <c r="C27" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="60" t="n">
+      <c r="D27" s="59" t="n">
         <v>44497</v>
       </c>
-      <c r="E27" s="60" t="n">
+      <c r="E27" s="59" t="n">
         <f aca="false">D27+4</f>
         <v>44501</v>
       </c>
@@ -4273,16 +4194,16 @@
     </row>
     <row r="28" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="60" t="n">
+      <c r="D28" s="59" t="n">
         <v>44494</v>
       </c>
-      <c r="E28" s="60" t="n">
+      <c r="E28" s="59" t="n">
         <f aca="false">D28+4</f>
         <v>44498</v>
       </c>
@@ -4367,16 +4288,16 @@
     </row>
     <row r="29" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="59" t="s">
+      <c r="C29" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="60" t="n">
+      <c r="D29" s="59" t="n">
         <v>44493</v>
       </c>
-      <c r="E29" s="60" t="n">
+      <c r="E29" s="59" t="n">
         <f aca="false">D29+2</f>
         <v>44495</v>
       </c>
@@ -4461,16 +4382,16 @@
     </row>
     <row r="30" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="60" t="n">
+      <c r="D30" s="59" t="n">
         <v>44502</v>
       </c>
-      <c r="E30" s="60" t="n">
+      <c r="E30" s="59" t="n">
         <f aca="false">D30+3</f>
         <v>44505</v>
       </c>
@@ -4555,16 +4476,16 @@
     </row>
     <row r="31" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="60" t="n">
+      <c r="D31" s="59" t="n">
         <v>44501</v>
       </c>
-      <c r="E31" s="60" t="n">
+      <c r="E31" s="59" t="n">
         <f aca="false">D31+4</f>
         <v>44505</v>
       </c>
@@ -4649,16 +4570,16 @@
     </row>
     <row r="32" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="59" t="s">
+      <c r="C32" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="60" t="n">
+      <c r="D32" s="59" t="n">
         <v>44500</v>
       </c>
-      <c r="E32" s="60" t="n">
+      <c r="E32" s="59" t="n">
         <f aca="false">D32+2</f>
         <v>44502</v>
       </c>
@@ -4743,16 +4664,16 @@
     </row>
     <row r="33" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="60" t="n">
+      <c r="D33" s="59" t="n">
         <v>44502</v>
       </c>
-      <c r="E33" s="60" t="n">
+      <c r="E33" s="59" t="n">
         <f aca="false">D33+3</f>
         <v>44505</v>
       </c>
@@ -4837,16 +4758,16 @@
     </row>
     <row r="34" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="60" t="n">
+      <c r="D34" s="59" t="n">
         <v>44502</v>
       </c>
-      <c r="E34" s="60" t="n">
+      <c r="E34" s="59" t="n">
         <f aca="false">D34+4</f>
         <v>44506</v>
       </c>
@@ -4931,16 +4852,16 @@
     </row>
     <row r="35" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="59" t="s">
+      <c r="C35" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="60" t="n">
+      <c r="D35" s="59" t="n">
         <v>44505</v>
       </c>
-      <c r="E35" s="60" t="n">
+      <c r="E35" s="59" t="n">
         <f aca="false">D35+2</f>
         <v>44507</v>
       </c>
@@ -5025,16 +4946,16 @@
     </row>
     <row r="36" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="60" t="n">
+      <c r="D36" s="59" t="n">
         <v>44501</v>
       </c>
-      <c r="E36" s="60" t="n">
+      <c r="E36" s="59" t="n">
         <f aca="false">D36+6</f>
         <v>44507</v>
       </c>
@@ -5119,16 +5040,16 @@
     </row>
     <row r="37" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
-      <c r="B37" s="61" t="s">
+      <c r="B37" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="59" t="s">
+      <c r="C37" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="60" t="n">
+      <c r="D37" s="59" t="n">
         <v>44507</v>
       </c>
-      <c r="E37" s="60" t="n">
+      <c r="E37" s="59" t="n">
         <f aca="false">D37+0</f>
         <v>44507</v>
       </c>
@@ -5213,12 +5134,12 @@
     </row>
     <row r="38" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="63"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
@@ -5300,16 +5221,16 @@
     </row>
     <row r="39" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="C39" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="68" t="n">
+      <c r="D39" s="67" t="n">
         <v>44515</v>
       </c>
-      <c r="E39" s="68" t="n">
+      <c r="E39" s="67" t="n">
         <f aca="false">D39+4</f>
         <v>44519</v>
       </c>
@@ -5394,16 +5315,16 @@
     </row>
     <row r="40" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="C40" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="68" t="n">
+      <c r="D40" s="67" t="n">
         <v>44515</v>
       </c>
-      <c r="E40" s="68" t="n">
+      <c r="E40" s="67" t="n">
         <f aca="false">D40+4</f>
         <v>44519</v>
       </c>
@@ -5488,16 +5409,16 @@
     </row>
     <row r="41" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
-      <c r="B41" s="66" t="s">
+      <c r="B41" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="67" t="s">
+      <c r="C41" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="68" t="n">
+      <c r="D41" s="67" t="n">
         <v>44515</v>
       </c>
-      <c r="E41" s="68" t="n">
+      <c r="E41" s="67" t="n">
         <f aca="false">D41+4</f>
         <v>44519</v>
       </c>
@@ -5582,16 +5503,16 @@
     </row>
     <row r="42" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="68" t="n">
+      <c r="D42" s="67" t="n">
         <v>44522</v>
       </c>
-      <c r="E42" s="68" t="n">
+      <c r="E42" s="67" t="n">
         <v>44522</v>
       </c>
       <c r="F42" s="38"/>
@@ -5675,16 +5596,16 @@
     </row>
     <row r="43" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="67" t="s">
+      <c r="C43" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="68" t="n">
+      <c r="D43" s="67" t="n">
         <v>44522</v>
       </c>
-      <c r="E43" s="68" t="n">
+      <c r="E43" s="67" t="n">
         <v>44522</v>
       </c>
       <c r="F43" s="38"/>
@@ -5768,16 +5689,16 @@
     </row>
     <row r="44" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
-      <c r="B44" s="66" t="s">
+      <c r="B44" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="67" t="s">
+      <c r="C44" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="68" t="n">
+      <c r="D44" s="67" t="n">
         <v>44523</v>
       </c>
-      <c r="E44" s="68" t="n">
+      <c r="E44" s="67" t="n">
         <v>44523</v>
       </c>
       <c r="F44" s="38"/>
@@ -5861,16 +5782,16 @@
     </row>
     <row r="45" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="67" t="s">
+      <c r="C45" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="68" t="n">
+      <c r="D45" s="67" t="n">
         <v>44525</v>
       </c>
-      <c r="E45" s="68" t="n">
+      <c r="E45" s="67" t="n">
         <v>44525</v>
       </c>
       <c r="F45" s="38"/>
@@ -5954,16 +5875,16 @@
     </row>
     <row r="46" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="67" t="s">
+      <c r="C46" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="68" t="n">
+      <c r="D46" s="67" t="n">
         <v>44524</v>
       </c>
-      <c r="E46" s="68" t="n">
+      <c r="E46" s="67" t="n">
         <v>44524</v>
       </c>
       <c r="F46" s="38"/>
@@ -6047,16 +5968,16 @@
     </row>
     <row r="47" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
-      <c r="B47" s="66" t="s">
+      <c r="B47" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="67" t="s">
+      <c r="C47" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="68" t="n">
+      <c r="D47" s="67" t="n">
         <v>44524</v>
       </c>
-      <c r="E47" s="68" t="n">
+      <c r="E47" s="67" t="n">
         <v>44524</v>
       </c>
       <c r="F47" s="38"/>
@@ -6140,16 +6061,16 @@
     </row>
     <row r="48" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
-      <c r="B48" s="66" t="s">
+      <c r="B48" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="68" t="n">
+      <c r="D48" s="67" t="n">
         <v>44523</v>
       </c>
-      <c r="E48" s="68" t="n">
+      <c r="E48" s="67" t="n">
         <v>44523</v>
       </c>
       <c r="F48" s="38"/>
@@ -6233,16 +6154,16 @@
     </row>
     <row r="49" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
-      <c r="B49" s="66" t="s">
+      <c r="B49" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="67" t="s">
+      <c r="C49" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="68" t="n">
+      <c r="D49" s="67" t="n">
         <v>44524</v>
       </c>
-      <c r="E49" s="68" t="n">
+      <c r="E49" s="67" t="n">
         <v>44524</v>
       </c>
       <c r="F49" s="38"/>
@@ -6326,16 +6247,16 @@
     </row>
     <row r="50" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
-      <c r="B50" s="66" t="s">
+      <c r="B50" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="67" t="s">
+      <c r="C50" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="68" t="n">
+      <c r="D50" s="67" t="n">
         <v>44525</v>
       </c>
-      <c r="E50" s="68" t="n">
+      <c r="E50" s="67" t="n">
         <v>44525</v>
       </c>
       <c r="F50" s="38"/>
@@ -6419,12 +6340,12 @@
     </row>
     <row r="51" s="40" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="72"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="70"/>
+      <c r="E51" s="71"/>
       <c r="F51" s="38"/>
       <c r="G51" s="38"/>
       <c r="H51" s="38"/>
@@ -6505,11 +6426,11 @@
       <c r="CE51" s="38"/>
     </row>
     <row r="53" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="73"/>
-      <c r="E53" s="74"/>
+      <c r="C53" s="72"/>
+      <c r="E53" s="73"/>
     </row>
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="75"/>
+      <c r="C54" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -6567,7 +6488,7 @@
       <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:BW6 BY6:CD6 M8:M51 AU51:AV51 CD7:CE51 AN51:AO51 S8:T51 Z51:AA51 AG51:AH51 BI51:BJ51 BP51:BQ51 BW51:BX51 G7:T7 U7:Y9 AB7:AF9 AI7:AM9 AP7:AT9 AW7:BA9 BD7:BH9 BK7:BO9 BR7:BV9 BY7:CC9 G9:O9 G8:M8 Q8:R8 Z18:AA18 AU38:AV38 AN38:AO38 U13:Y14 AB11:AF12 AI11:AM17 AP11:AT17 AW11:BA17 BD11:BH17 BK11:BO17 BR11:BV17 Z38:AA38 Z19:Z37 AB19:AF37 AI19:AM19 AP20:AT21 AW19:BA21 BE19:BH37 BK19:BO37 BR19:BV37 AG7:AH38 BI7:BJ38 BP7:BQ38 BW7:BX38 Z39:Z50 AP39:AT50 AW39:BA50 AB39:AM50 BD50:BT50 Y11 U11:U12 AB15:AF15 AE13:AF13 AF14 U16:Y17 U15:V15 AB17:AE17 AC16:AF16 AI22:AM37 AI21 AM21 AI20:AJ20 AS19:AT19 AW24:BA26 AP23:AT23 AP22:AR22 AZ23:BA23 AP25:AR25 AT24 AP27:AR27 AW28:BA29 AX27:BA27 AP26 AT26 AW37:BA37 AY32:BA32 AW30 AR29:AT29 AW33:AW34 AP30:AT37 AW35:AZ35 BD39:BJ41 BP39:BX41 BD42:BQ43 BU43:BX43 BD44:BR44 BT44:BX44 BD45:BT45 BV45:BX45 BD46:BS47 BW47:BX47 BD48:BR48 BT48:BX48 BD49:BS49 BU49:BX49 BV50:BX50 BD19:BD35 BW46:BX46 BU42:BX42">
+  <conditionalFormatting sqref="G6:BW6 BY6:CD6 M8:M51 AU51:AV51 CD7:CE51 AN51:AO51 S8:T51 Z51:AA51 AG51:AH51 BI51:BJ51 BP51:BQ51 BW51:BX51 G7:T7 U7:Y8 AB7:AF9 AI7:AM9 AP7:AT9 AW7:BA9 BD7:BH9 BK7:BO9 BR7:BV9 BY7:CC9 G9:O9 G8:M8 Q8:R8 Z18:AA18 AU38:AV38 AN38:AO38 U13:Y14 AB11:AF12 AI11:AM17 AP11:AT17 AW11:BA17 BD11:BH17 BK11:BO17 BR11:BV17 Z38:AA38 Z19:Z37 AB19:AF37 AI19:AM19 AP20:AT21 AW19:BA21 BE19:BH37 BK19:BO37 BR19:BV37 AG7:AH38 BI7:BJ38 BP7:BQ38 BW7:BX38 Z39:Z50 AP39:AT50 AW39:BA50 AB39:AM50 BD50:BT50 Y11 U11:U12 AB15:AF15 AE13:AF13 AF14 U16:Y17 U15:V15 AB17:AE17 AC16:AF16 AI22:AM37 AI21 AM21 AI20:AJ20 AS19:AT19 AW24:BA26 AP23:AT23 AP22:AR22 AZ23:BA23 AP25:AR25 AT24 AP27:AR27 AW28:BA29 AX27:BA27 AP26 AT26 AW37:BA37 AY32:BA32 AW30 AR29:AT29 AW33:AW34 AP30:AT37 AW35:AZ35 BD39:BJ41 BP39:BX41 BD42:BQ43 BU43:BX43 BD44:BR44 BT44:BX44 BD45:BT45 BV45:BX45 BD46:BS47 BW47:BX47 BD48:BR48 BT48:BX48 BD49:BS49 BU49:BX49 BV50:BX50 BD19:BD35 BW46:BX46 BU42:BX42 V9:Y9">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
@@ -6575,14 +6496,14 @@
       <formula>AND(task_end&gt;=G$5,task_start&lt;H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:BW6 BY6:CD6 M8:M51 AU51:AV51 CD7:CE51 AN51:AO51 S8:T51 Z51:AA51 AG51:AH51 BI51:BJ51 BP51:BQ51 BW51:BX51 G7:T7 U7:Y9 AB7:AF9 AI7:AM9 AP7:AT9 AW7:BA9 BD7:BH9 BK7:BO9 BR7:BV9 BY7:CC9 G9:O9 G8:M8 Q8:R8 Z18:AA18 AU38:AV38 AN38:AO38 U13:Y14 AB11:AF12 AI11:AM17 AP11:AT17 AW11:BA17 BD11:BH17 BK11:BO17 BR11:BV17 Z38:AA38 Z19:Z37 AB19:AF37 AI19:AM19 AP20:AT21 AW19:BA21 BE19:BH37 BK19:BO37 BR19:BV37 AG7:AH38 BI7:BJ38 BP7:BQ38 BW7:BX38 Z39:Z50 AP39:AT50 AW39:BA50 AB39:AM50 BD50:BT50 Y11 U11:U12 AB15:AF15 AE13:AF13 AF14 U16:Y17 U15:V15 AB17:AE17 AC16:AF16 AI22:AM37 AI21 AM21 AI20:AJ20 AS19:AT19 AW24:BA26 AP23:AT23 AP22:AR22 AZ23:BA23 AP25:AR25 AT24 AP27:AR27 AW28:BA29 AX27:BA27 AP26 AT26 AW37:BA37 AY32:BA32 AW30 AR29:AT29 AW33:AW34 AP30:AT37 AW35:AZ35 BD39:BJ41 BP39:BX41 BD42:BQ43 BU43:BX43 BD44:BR44 BT44:BX44 BD45:BT45 BV45:BX45 BD46:BS47 BW47:BX47 BD48:BR48 BT48:BX48 BD49:BS49 BU49:BX49 BV50:BX50 BD19:BD35 BW46:BX46 BU42:BX42">
+  <conditionalFormatting sqref="G5:BW6 BY6:CD6 M8:M51 AU51:AV51 CD7:CE51 AN51:AO51 S8:T51 Z51:AA51 AG51:AH51 BI51:BJ51 BP51:BQ51 BW51:BX51 G7:T7 U7:Y8 AB7:AF9 AI7:AM9 AP7:AT9 AW7:BA9 BD7:BH9 BK7:BO9 BR7:BV9 BY7:CC9 G9:O9 G8:M8 Q8:R8 Z18:AA18 AU38:AV38 AN38:AO38 U13:Y14 AB11:AF12 AI11:AM17 AP11:AT17 AW11:BA17 BD11:BH17 BK11:BO17 BR11:BV17 Z38:AA38 Z19:Z37 AB19:AF37 AI19:AM19 AP20:AT21 AW19:BA21 BE19:BH37 BK19:BO37 BR19:BV37 AG7:AH38 BI7:BJ38 BP7:BQ38 BW7:BX38 Z39:Z50 AP39:AT50 AW39:BA50 AB39:AM50 BD50:BT50 Y11 U11:U12 AB15:AF15 AE13:AF13 AF14 U16:Y17 U15:V15 AB17:AE17 AC16:AF16 AI22:AM37 AI21 AM21 AI20:AJ20 AS19:AT19 AW24:BA26 AP23:AT23 AP22:AR22 AZ23:BA23 AP25:AR25 AT24 AP27:AR27 AW28:BA29 AX27:BA27 AP26 AT26 AW37:BA37 AY32:BA32 AW30 AR29:AT29 AW33:AW34 AP30:AT37 AW35:AZ35 BD39:BJ41 BP39:BX41 BD42:BQ43 BU43:BX43 BD44:BR44 BT44:BX44 BD45:BT45 BV45:BX45 BD46:BS47 BW47:BX47 BD48:BR48 BT48:BX48 BD49:BS49 BU49:BX49 BV50:BX50 BD19:BD35 BW46:BX46 BU42:BX42 V9:Y9">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BY5:CE5 BX5:BX6 CE6">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
-      <formula>AND(TODAY()&gt;=BX$5,TODAY(&lt;#ref!)</formula>
+      <formula>AND(TODAY()&gt;=BX$5,TODAY(&lt;#ref!))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX6 CE6">
@@ -6763,13 +6684,11 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.347222222222222" header="0.511811023622047" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="true" differentOddEven="false">
+  <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.347222222222222" header="0.511805555555555" footer="0.3"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
-    <firstHeader/>
-    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>